<commit_message>
ExtractSREO.py changed to fileExtraction.py, cleaned up code
</commit_message>
<xml_diff>
--- a/ExtractSREO/Standardized-2021 12 14_MWest_Debt Schedule.xlsx
+++ b/ExtractSREO/Standardized-2021 12 14_MWest_Debt Schedule.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W35"/>
+  <dimension ref="A1:W34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1417,11 +1417,7 @@
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr">
-        <is>
-          <t>9/9/2019</t>
-        </is>
-      </c>
+      <c r="I16" t="inlineStr"/>
       <c r="J16" t="inlineStr">
         <is>
           <t xml:space="preserve"> Invesco CMI Investments, L.P. </t>
@@ -2162,7 +2158,7 @@
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>9.40409E+13</t>
+          <t>9.40E+13</t>
         </is>
       </c>
       <c r="N27" t="inlineStr"/>
@@ -2227,7 +2223,7 @@
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>9.40412E+13</t>
+          <t>9.40E+13</t>
         </is>
       </c>
       <c r="N28" t="inlineStr"/>
@@ -2292,7 +2288,7 @@
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>9.40412E+13</t>
+          <t>9.40E+13</t>
         </is>
       </c>
       <c r="N29" t="inlineStr"/>
@@ -2418,7 +2414,7 @@
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>9.40412E+13</t>
+          <t>9.40E+13</t>
         </is>
       </c>
       <c r="N31" t="inlineStr"/>
@@ -2483,7 +2479,7 @@
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>9.40409E+13</t>
+          <t>9.40E+13</t>
         </is>
       </c>
       <c r="N32" t="inlineStr"/>
@@ -2548,7 +2544,7 @@
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>9.40412E+13</t>
+          <t>9.40E+13</t>
         </is>
       </c>
       <c r="N33" t="inlineStr"/>
@@ -2613,7 +2609,7 @@
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>9.405E+13</t>
+          <t>9.41E+13</t>
         </is>
       </c>
       <c r="N34" t="inlineStr"/>
@@ -2639,35 +2635,6 @@
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr"/>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
-      <c r="G35" t="inlineStr"/>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr"/>
-      <c r="J35" t="inlineStr"/>
-      <c r="K35" t="inlineStr"/>
-      <c r="L35" t="inlineStr"/>
-      <c r="M35" t="inlineStr"/>
-      <c r="N35" t="inlineStr"/>
-      <c r="O35" t="inlineStr"/>
-      <c r="P35" t="inlineStr"/>
-      <c r="Q35" t="inlineStr"/>
-      <c r="R35" t="inlineStr"/>
-      <c r="S35" t="inlineStr"/>
-      <c r="T35" t="inlineStr"/>
-      <c r="U35" t="inlineStr"/>
-      <c r="V35" t="inlineStr"/>
-      <c r="W35" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>